<commit_message>
Updated dual motor driver and file organization
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28280" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tilty Duo BT" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="157">
   <si>
     <t>Part</t>
   </si>
@@ -415,15 +415,6 @@
     <t>150 Ω Resistor</t>
   </si>
   <si>
-    <t>68 Ω Resistor</t>
-  </si>
-  <si>
-    <t>R3, R8</t>
-  </si>
-  <si>
-    <t>RC0603JR-0768RL</t>
-  </si>
-  <si>
     <t>SOT23-5L</t>
   </si>
   <si>
@@ -479,6 +470,30 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>R3, R6, R8</t>
+  </si>
+  <si>
+    <t>1622866-1</t>
+  </si>
+  <si>
+    <t>RMCF0603FT1K00</t>
+  </si>
+  <si>
+    <t>RC1608F680CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF0603FT68R0 </t>
+  </si>
+  <si>
+    <t>68 Ω Resistor (1%)</t>
+  </si>
+  <si>
+    <t>1K Ω Resistor (1%)</t>
+  </si>
+  <si>
+    <t>LTST-C171KGKT</t>
   </si>
 </sst>
 </file>
@@ -576,10 +591,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -747,7 +832,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="173">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -800,6 +885,41 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -850,6 +970,41 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2235,7 +2390,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B29" s="9"/>
       <c r="D29" s="5"/>
@@ -2573,7 +2728,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="B11:B12 B14:B24" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -3593,7 +3747,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B32" s="9"/>
       <c r="D32" s="5"/>
@@ -3871,7 +4025,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="B13:B21" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -3885,10 +4038,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:J7"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4242,13 +4395,13 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -4257,7 +4410,7 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G8" s="2">
         <v>0.28999999999999998</v>
@@ -4278,7 +4431,7 @@
         <v>46</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N8" s="17">
         <v>0.22</v>
@@ -4483,7 +4636,7 @@
         <v>126</v>
       </c>
       <c r="N14" s="11">
-        <v>0.39900000000000002</v>
+        <v>3.9899999999999998E-2</v>
       </c>
       <c r="O14" s="10">
         <v>6000</v>
@@ -4527,7 +4680,15 @@
       <c r="K15" s="2">
         <v>0.14580000000000001</v>
       </c>
-      <c r="O15" s="10"/>
+      <c r="M15" t="s">
+        <v>156</v>
+      </c>
+      <c r="N15" s="12">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="O15" s="10">
+        <v>6000</v>
+      </c>
       <c r="Q15" s="15">
         <f>D15*J15</f>
         <v>0.26700000000000002</v>
@@ -4685,7 +4846,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>43</v>
@@ -4700,31 +4861,31 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="G20" s="2">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="H20" s="2">
-        <v>1.7000000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I20" s="2">
-        <v>1.7000000000000001E-2</v>
+        <v>5.1999999999999998E-3</v>
       </c>
       <c r="J20" s="2">
-        <v>9.1999999999999998E-3</v>
+        <v>3.8E-3</v>
       </c>
       <c r="K20" s="2">
-        <v>7.0000000000000001E-3</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="L20" t="s">
         <v>46</v>
       </c>
       <c r="M20" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="N20" s="11">
-        <v>1.6000000000000001E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="O20" s="10">
         <v>5000</v>
@@ -4732,118 +4893,131 @@
       <c r="P20" s="18"/>
       <c r="Q20" s="15">
         <f>J20*D20</f>
-        <v>1.84E-2</v>
+        <v>7.6E-3</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="D21" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="G21" s="2">
         <v>0.1</v>
       </c>
       <c r="H21" s="2">
-        <v>0.01</v>
+        <v>1.4E-2</v>
       </c>
       <c r="I21" s="2">
-        <v>8.0000000000000002E-3</v>
+        <v>1.04E-2</v>
       </c>
       <c r="J21" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="K21" s="2">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="10"/>
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" t="s">
+        <v>153</v>
+      </c>
+      <c r="N21" s="11">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="O21" s="10">
+        <v>5000</v>
+      </c>
       <c r="P21" s="18"/>
-      <c r="Q21" s="15"/>
+      <c r="Q21" s="15">
+        <f>J21*D21</f>
+        <v>2.4E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="16"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="15"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="5">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="I22" s="2">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="J22" s="2">
-        <v>9.1999999999999998E-3</v>
-      </c>
-      <c r="K22" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="F23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.32E-2</v>
+      </c>
+      <c r="L23" t="s">
         <v>46</v>
       </c>
-      <c r="M22" t="s">
-        <v>62</v>
-      </c>
-      <c r="N22" s="11">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="O22" s="10">
-        <v>5000</v>
-      </c>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="15">
-        <f>D22*J22</f>
-        <v>9.1999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="B23" s="16"/>
-      <c r="O23" s="10"/>
+      <c r="M23" t="s">
+        <v>137</v>
+      </c>
+      <c r="N23" s="11">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="O23" s="10">
+        <v>4000</v>
+      </c>
       <c r="P23" s="18"/>
-      <c r="Q23" s="15"/>
+      <c r="Q23" s="15">
+        <f>D23*J23</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="D24" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -4855,16 +5029,16 @@
         <v>0.1</v>
       </c>
       <c r="H24" s="2">
-        <v>2.9000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="I24" s="2">
-        <v>2.0400000000000001E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="J24" s="2">
-        <v>1.5599999999999999E-2</v>
+        <v>1.0200000000000001E-2</v>
       </c>
       <c r="K24" s="2">
-        <v>1.32E-2</v>
+        <v>8.6E-3</v>
       </c>
       <c r="L24" t="s">
         <v>46</v>
@@ -4873,130 +5047,130 @@
         <v>140</v>
       </c>
       <c r="N24" s="11">
-        <v>2.0999999999999999E-3</v>
+        <v>1.4E-3</v>
       </c>
       <c r="O24" s="10">
-        <v>4000</v>
+        <v>15000</v>
       </c>
       <c r="P24" s="18"/>
       <c r="Q24" s="15">
         <f>D24*J24</f>
-        <v>1.5599999999999999E-2</v>
+        <v>5.1000000000000004E-2</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D25" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="G25" s="2">
         <v>0.1</v>
       </c>
       <c r="H25" s="2">
-        <v>1.9E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="I25" s="2">
-        <v>1.32E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="J25" s="2">
-        <v>1.0200000000000001E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="K25" s="2">
-        <v>8.6E-3</v>
+        <v>2.86E-2</v>
       </c>
       <c r="L25" t="s">
         <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>143</v>
+        <v>78</v>
       </c>
       <c r="N25" s="11">
-        <v>1.4E-3</v>
+        <v>9.1999999999999998E-3</v>
       </c>
       <c r="O25" s="10">
-        <v>15000</v>
+        <v>4000</v>
       </c>
       <c r="P25" s="18"/>
       <c r="Q25" s="15">
-        <f>D25*J25</f>
-        <v>5.1000000000000004E-2</v>
+        <f>J25*D25</f>
+        <v>0.186</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="D26" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="G26" s="2">
         <v>0.1</v>
       </c>
       <c r="H26" s="2">
-        <v>6.2E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="I26" s="2">
-        <v>6.2E-2</v>
+        <v>2.4400000000000002E-2</v>
       </c>
       <c r="J26" s="2">
-        <v>6.2E-2</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="K26" s="2">
-        <v>2.86E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="L26" t="s">
         <v>46</v>
       </c>
       <c r="M26" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="N26" s="11">
-        <v>9.1999999999999998E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="O26" s="10">
         <v>4000</v>
       </c>
       <c r="P26" s="18"/>
       <c r="Q26" s="15">
-        <f>J26*D26</f>
-        <v>0.186</v>
+        <f>D26*J26</f>
+        <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -5005,31 +5179,31 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G27" s="2">
         <v>0.1</v>
       </c>
       <c r="H27" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4.02E-2</v>
+      </c>
+      <c r="K27" s="2">
         <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="I27" s="2">
-        <v>2.4400000000000002E-2</v>
-      </c>
-      <c r="J27" s="2">
-        <v>1.8599999999999998E-2</v>
-      </c>
-      <c r="K27" s="2">
-        <v>1.5800000000000002E-2</v>
       </c>
       <c r="L27" t="s">
         <v>46</v>
       </c>
       <c r="M27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N27" s="11">
-        <v>4.1999999999999997E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="O27" s="10">
         <v>4000</v>
@@ -5037,118 +5211,81 @@
       <c r="P27" s="18"/>
       <c r="Q27" s="15">
         <f>D27*J27</f>
-        <v>1.8599999999999998E-2</v>
+        <v>4.02E-2</v>
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H28" s="2">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="I28" s="2">
-        <v>5.2400000000000002E-2</v>
-      </c>
-      <c r="J28" s="2">
-        <v>4.02E-2</v>
-      </c>
-      <c r="K28" s="2">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="L28" t="s">
-        <v>46</v>
-      </c>
-      <c r="M28" t="s">
-        <v>139</v>
-      </c>
-      <c r="N28" s="11">
-        <v>1.1299999999999999E-2</v>
-      </c>
-      <c r="O28" s="10">
-        <v>4000</v>
-      </c>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="15">
-        <f>D28*J28</f>
-        <v>4.02E-2</v>
-      </c>
+      <c r="B28" s="9"/>
+      <c r="D28" s="5"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="10"/>
     </row>
     <row r="29" spans="1:17">
       <c r="B29" s="9"/>
-      <c r="D29" s="5"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="10"/>
+      <c r="Q29" s="15">
+        <f>SUM(Q2:Q27)</f>
+        <v>17.470199999999998</v>
+      </c>
     </row>
     <row r="30" spans="1:17">
       <c r="B30" s="9"/>
-      <c r="Q30" s="15">
-        <f>SUM(Q2:Q28)</f>
-        <v>17.466199999999997</v>
-      </c>
+      <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="B31" s="9"/>
-      <c r="L31" s="6"/>
+      <c r="A31" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="28">
+        <v>37</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q31" s="15">
+        <f>Q29+17.1</f>
+        <v>34.5702</v>
+      </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="28">
-        <v>37</v>
+        <v>112</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>143</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q32" s="15">
-        <f>Q30+17.1</f>
-        <v>34.566199999999995</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+        <f>Q31+18.21</f>
+        <v>52.780200000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="P33" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q33" s="15">
-        <f>Q32+18.21</f>
-        <v>52.776199999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
+        <v>116</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="10"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="D34" s="5"/>
       <c r="G34" s="2"/>
@@ -5158,12 +5295,12 @@
       <c r="N34" s="11"/>
       <c r="O34" s="10"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:15">
       <c r="A35" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="D35" s="5"/>
       <c r="G35" s="2"/>
@@ -5173,13 +5310,8 @@
       <c r="N35" s="11"/>
       <c r="O35" s="10"/>
     </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>117</v>
-      </c>
+    <row r="36" spans="1:15">
+      <c r="B36" s="9"/>
       <c r="D36" s="5"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -5188,7 +5320,7 @@
       <c r="N36" s="11"/>
       <c r="O36" s="10"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:15">
       <c r="B37" s="9"/>
       <c r="D37" s="5"/>
       <c r="G37" s="2"/>
@@ -5198,7 +5330,7 @@
       <c r="N37" s="11"/>
       <c r="O37" s="10"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:15">
       <c r="B38" s="9"/>
       <c r="D38" s="5"/>
       <c r="G38" s="2"/>
@@ -5208,7 +5340,7 @@
       <c r="N38" s="11"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:15">
       <c r="B39" s="9"/>
       <c r="D39" s="5"/>
       <c r="G39" s="2"/>
@@ -5218,7 +5350,7 @@
       <c r="N39" s="11"/>
       <c r="O39" s="10"/>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:15">
       <c r="B40" s="9"/>
       <c r="D40" s="5"/>
       <c r="G40" s="2"/>
@@ -5228,7 +5360,7 @@
       <c r="N40" s="11"/>
       <c r="O40" s="10"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:15">
       <c r="B41" s="9"/>
       <c r="D41" s="5"/>
       <c r="G41" s="2"/>
@@ -5238,7 +5370,7 @@
       <c r="N41" s="11"/>
       <c r="O41" s="10"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:15">
       <c r="B42" s="9"/>
       <c r="D42" s="5"/>
       <c r="G42" s="2"/>
@@ -5248,7 +5380,7 @@
       <c r="N42" s="11"/>
       <c r="O42" s="10"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:15">
       <c r="B43" s="9"/>
       <c r="D43" s="5"/>
       <c r="G43" s="2"/>
@@ -5258,7 +5390,7 @@
       <c r="N43" s="11"/>
       <c r="O43" s="10"/>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:15">
       <c r="B44" s="9"/>
       <c r="D44" s="5"/>
       <c r="G44" s="2"/>
@@ -5268,7 +5400,7 @@
       <c r="N44" s="11"/>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:15">
       <c r="B45" s="9"/>
       <c r="D45" s="5"/>
       <c r="G45" s="2"/>
@@ -5278,7 +5410,7 @@
       <c r="N45" s="11"/>
       <c r="O45" s="10"/>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:15">
       <c r="B46" s="9"/>
       <c r="D46" s="5"/>
       <c r="G46" s="2"/>
@@ -5288,7 +5420,7 @@
       <c r="N46" s="11"/>
       <c r="O46" s="10"/>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:15">
       <c r="B47" s="9"/>
       <c r="D47" s="5"/>
       <c r="G47" s="2"/>
@@ -5298,7 +5430,7 @@
       <c r="N47" s="11"/>
       <c r="O47" s="10"/>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:15">
       <c r="B48" s="9"/>
       <c r="D48" s="5"/>
       <c r="G48" s="2"/>
@@ -5379,7 +5511,6 @@
       <c r="O55" s="10"/>
     </row>
     <row r="56" spans="2:15">
-      <c r="B56" s="9"/>
       <c r="D56" s="5"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -5394,7 +5525,6 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="N57" s="11"/>
       <c r="O57" s="10"/>
     </row>
     <row r="58" spans="2:15">
@@ -5403,7 +5533,6 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
-      <c r="O58" s="10"/>
     </row>
     <row r="59" spans="2:15">
       <c r="D59" s="5"/>
@@ -5434,22 +5563,15 @@
       <c r="J62" s="2"/>
     </row>
     <row r="63" spans="2:15">
-      <c r="D63" s="5"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="2:15">
-      <c r="D64" s="3"/>
+      <c r="D63" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B22:B23 B34 B36 B18 B19:B20 B25:B26" numberStoredAsText="1"/>
-    <ignoredError sqref="Q26 Q20 Q11 Q4" formula="1"/>
-    <ignoredError sqref="Q30" emptyCellReference="1"/>
+    <ignoredError sqref="B22 B33 B35 B18 B19:B20 B24:B25" numberStoredAsText="1"/>
+    <ignoredError sqref="Q25 Q20 Q11 Q4" formula="1"/>
+    <ignoredError sqref="Q29" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5464,7 +5586,7 @@
   <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5775,13 +5897,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
@@ -5790,7 +5912,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G7" s="2">
         <v>0.28999999999999998</v>
@@ -5811,7 +5933,7 @@
         <v>46</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N7" s="17">
         <v>0.22</v>
@@ -6275,7 +6397,7 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G21" s="2">
         <v>0.1</v>
@@ -6296,7 +6418,7 @@
         <v>46</v>
       </c>
       <c r="M21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N21" s="11">
         <v>2.0999999999999999E-3</v>
@@ -6318,7 +6440,7 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D22" s="5">
         <v>5</v>
@@ -6327,7 +6449,7 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G22" s="2">
         <v>0.1</v>
@@ -6348,7 +6470,7 @@
         <v>46</v>
       </c>
       <c r="M22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N22" s="11">
         <v>1.4E-3</v>
@@ -6370,7 +6492,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D23" s="5">
         <v>2</v>
@@ -6431,7 +6553,7 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G24" s="2">
         <v>0.1</v>
@@ -6452,7 +6574,7 @@
         <v>46</v>
       </c>
       <c r="M24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N24" s="11">
         <v>4.1999999999999997E-3</v>
@@ -6483,7 +6605,7 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G25" s="2">
         <v>0.1</v>
@@ -6504,7 +6626,7 @@
         <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N25" s="11">
         <v>1.1299999999999999E-2</v>
@@ -6547,7 +6669,7 @@
         <v>31</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Q29" s="15">
         <f>Q27+17.1</f>
@@ -6559,10 +6681,10 @@
         <v>112</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="Q30" s="15">
         <f>Q29+18.21</f>
@@ -6589,7 +6711,7 @@
         <v>114</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D32" s="5"/>
       <c r="G32" s="2"/>
@@ -6655,6 +6777,9 @@
       <c r="O37" s="10"/>
     </row>
     <row r="38" spans="1:15">
+      <c r="A38" s="39" t="s">
+        <v>146</v>
+      </c>
       <c r="B38" s="9"/>
       <c r="D38" s="5"/>
       <c r="G38" s="2"/>

</xml_diff>

<commit_message>
Updated dual motor driver and Tilty Duo/Quad PCBs, added a copuple experimental arduino programs
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tilty Duo BT" sheetId="1" r:id="rId1"/>
@@ -4041,7 +4041,7 @@
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5567,7 +5567,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="B22 B33 B35 B18 B19:B20 B24:B25" numberStoredAsText="1"/>
     <ignoredError sqref="Q25 Q20 Q11 Q4" formula="1"/>

</xml_diff>